<commit_message>
Streamlined the hierachy and removed some bugs with parents
</commit_message>
<xml_diff>
--- a/forms/contact/chp-create.xlsx
+++ b/forms/contact/chp-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="292">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -150,6 +150,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लग इन गरेको प्रयोगकर्ताको सम्पर्क </t>
     </r>
@@ -180,6 +181,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लॉग इन यूज़र के स्थान का </t>
     </r>
@@ -207,6 +209,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">लग इन गरेको प्रयोगकर्ताको स्थानको </t>
     </r>
@@ -252,39 +255,6 @@
     <t xml:space="preserve">Cannot be inside the person group without having all fields saved to person. And needs separate db-objects because cannot have one that handles the different place types. Last part is now incorrect... as long as it is read only it could be a string of appearance db-object and work fine.</t>
   </si>
   <si>
-    <t xml:space="preserve">parent_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belongs To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">यह व्यक्ति इस जगह से जुड़ा है</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orang ini terhubung ke tempat ini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ni wa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">यो व्यक्ति यस ठाउँसँग सम्बन्धित छ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Associé avec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db-object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${parent}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${type_label}</t>
-  </si>
-  <si>
     <t xml:space="preserve">hidden</t>
   </si>
   <si>
@@ -306,7 +276,10 @@
     <t xml:space="preserve">jr:choice-name(${type_selector},'${type_selector}')</t>
   </si>
   <si>
-    <t xml:space="preserve">person</t>
+    <t xml:space="preserve">chp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New CHP</t>
   </si>
   <si>
     <t xml:space="preserve">parent</t>
@@ -321,6 +294,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">मूल </t>
     </r>
@@ -363,6 +337,9 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
+    <t xml:space="preserve">person</t>
+  </si>
+  <si>
     <t xml:space="preserve">Full name</t>
   </si>
   <si>
@@ -550,6 +527,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">कृपया एक सही स्थानीय नंबर दर्ज करें</t>
     </r>
@@ -569,6 +547,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">या मानक अंतरराष्ट्रीय प्रारूप का उपयोग करें</t>
     </r>
@@ -588,6 +567,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">जिसमें एक प्लस साइन </t>
     </r>
@@ -607,6 +587,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">और देश कोड शामिल है। उदाहरण के लिए</t>
     </r>
@@ -721,6 +702,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहरी </t>
     </r>
@@ -748,6 +730,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहिरी </t>
     </r>
@@ -793,7 +776,7 @@
     <t xml:space="preserve">create</t>
   </si>
   <si>
-    <t xml:space="preserve">${phone} != '' and (selected( ${role},'chw') or selected( ${role},'chw_supervisor'))</t>
+    <t xml:space="preserve">${phone} != '' and (selected( ${role},'chp') or selected( ${role},'chp_supervisor'))</t>
   </si>
   <si>
     <t xml:space="preserve">meta</t>
@@ -823,6 +806,9 @@
     <t xml:space="preserve">yes_no</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
@@ -973,9 +959,6 @@
     <t xml:space="preserve">roles</t>
   </si>
   <si>
-    <t xml:space="preserve">chp</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHP</t>
   </si>
   <si>
@@ -994,84 +977,6 @@
     <t xml:space="preserve">ASC</t>
   </si>
   <si>
-    <t xml:space="preserve">chp_supervisor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHP Supervisor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">सामुदायिक स्वास्थ्यकर्मी के मैनेजर</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kader Pengawas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mkuu wa wahudumu wa afya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">महिला स्वास्थ्य स्वयम् सेविकाको सुपरभाइजर</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Superviseur ASC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nurse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">नर्स</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perawat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muuguzi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infirmier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">स्वास्थ्य केंद्र के मैनजर</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manajer Fasilitas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meneja wa Kituo cha afya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">स्वास्थ्य संस्था प्रमुख</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personnel médical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">मरीज़ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mgonjwa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">बिरामी</t>
-  </si>
-  <si>
     <t xml:space="preserve">other</t>
   </si>
   <si>
@@ -1159,6 +1064,12 @@
     <t xml:space="preserve">Zone</t>
   </si>
   <si>
+    <t xml:space="preserve">community_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
@@ -1175,9 +1086,6 @@
   </si>
   <si>
     <t xml:space="preserve">default_language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New CHP</t>
   </si>
   <si>
     <t xml:space="preserve">contact:chp:create</t>
@@ -1232,6 +1140,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1353,11 +1262,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1369,43 +1278,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1413,47 +1322,47 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1477,15 +1386,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1497,11 +1406,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1589,7 +1498,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1605,7 +1514,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.3"/>
@@ -2187,39 +2097,19 @@
       <c r="AR9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>63</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="13" t="s">
-        <v>64</v>
-      </c>
+      <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>66</v>
-      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
@@ -2228,29 +2118,15 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
-      <c r="V10" s="13" t="s">
-        <v>67</v>
-      </c>
+      <c r="V10" s="13"/>
       <c r="W10" s="13"/>
-      <c r="X10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB10" s="13" t="s">
-        <v>68</v>
-      </c>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
-      <c r="AD10" s="13" t="s">
-        <v>68</v>
-      </c>
+      <c r="AD10" s="13"/>
       <c r="AE10" s="13"/>
       <c r="AF10" s="13"/>
       <c r="AG10" s="13"/>
@@ -2295,7 +2171,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -2359,7 +2235,7 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -2396,10 +2272,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>33</v>
@@ -2423,7 +2299,7 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -2435,7 +2311,7 @@
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="15" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
@@ -2462,10 +2338,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -2487,7 +2363,7 @@
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
@@ -2586,10 +2462,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>33</v>
@@ -2645,27 +2521,27 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>79</v>
-      </c>
       <c r="E18" s="21" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
@@ -2689,7 +2565,7 @@
       <c r="AC18" s="21"/>
       <c r="AD18" s="21"/>
       <c r="AE18" s="21" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="AF18" s="21"/>
       <c r="AG18" s="21"/>
@@ -2707,27 +2583,27 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
@@ -2751,7 +2627,7 @@
       <c r="AC19" s="21"/>
       <c r="AD19" s="21"/>
       <c r="AE19" s="21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AF19" s="21"/>
       <c r="AG19" s="21"/>
@@ -2775,26 +2651,26 @@
         <v>1</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H20" s="21"/>
       <c r="I20" s="21" t="s">
         <v>54</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
@@ -2879,10 +2755,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -2892,7 +2768,7 @@
       <c r="H22" s="21"/>
       <c r="I22" s="26"/>
       <c r="J22" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
@@ -2906,7 +2782,7 @@
       <c r="T22" s="21"/>
       <c r="U22" s="21"/>
       <c r="V22" s="21" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="W22" s="21"/>
       <c r="X22" s="21"/>
@@ -2933,10 +2809,10 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="21"/>
@@ -2958,7 +2834,7 @@
       <c r="T23" s="21"/>
       <c r="U23" s="21"/>
       <c r="V23" s="21" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="W23" s="21"/>
       <c r="X23" s="21"/>
@@ -2988,7 +2864,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>33</v>
@@ -3037,13 +2913,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -3052,18 +2928,18 @@
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="K25" s="21" t="s">
-        <v>102</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
@@ -3074,7 +2950,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
       <c r="X25" s="21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="Y25" s="21"/>
       <c r="Z25" s="21"/>
@@ -3099,13 +2975,13 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -3115,7 +2991,7 @@
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
       <c r="K26" s="21" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -3153,13 +3029,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -3168,18 +3044,18 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
       <c r="N27" s="21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="P27" s="21"/>
       <c r="Q27" s="21"/>
@@ -3213,13 +3089,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -3229,15 +3105,15 @@
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
       <c r="K28" s="21" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="P28" s="21"/>
       <c r="Q28" s="21"/>
@@ -3271,13 +3147,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -3288,7 +3164,7 @@
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
       <c r="L29" s="21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="M29" s="21"/>
       <c r="N29" s="21"/>
@@ -3325,10 +3201,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="21"/>
@@ -3350,7 +3226,7 @@
       <c r="T30" s="21"/>
       <c r="U30" s="21"/>
       <c r="V30" s="26" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="W30" s="21"/>
       <c r="X30" s="21"/>
@@ -3377,10 +3253,10 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -3402,7 +3278,7 @@
       <c r="T31" s="26"/>
       <c r="U31" s="21"/>
       <c r="V31" s="27" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
@@ -3429,10 +3305,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="21"/>
@@ -3454,7 +3330,7 @@
       <c r="T32" s="21"/>
       <c r="U32" s="21"/>
       <c r="V32" s="21" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="W32" s="21"/>
       <c r="X32" s="21"/>
@@ -3481,13 +3357,13 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
@@ -3583,36 +3459,36 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H35" s="21"/>
       <c r="I35" s="21" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K35" s="21"/>
       <c r="L35" s="21" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
@@ -3649,49 +3525,49 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="21" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="P36" s="29" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Q36" s="21"/>
       <c r="R36" s="21"/>
       <c r="S36" s="21"/>
       <c r="T36" s="21"/>
       <c r="U36" s="21" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="V36" s="21"/>
       <c r="W36" s="21"/>
@@ -3719,49 +3595,49 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="21"/>
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
       <c r="N37" s="21" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="P37" s="29" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
       <c r="S37" s="21"/>
       <c r="T37" s="21"/>
       <c r="U37" s="21" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="V37" s="21"/>
       <c r="W37" s="21"/>
@@ -3789,29 +3665,29 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H38" s="21"/>
       <c r="I38" s="21" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="J38" s="21"/>
       <c r="K38" s="21"/>
@@ -3828,23 +3704,23 @@
       <c r="V38" s="21"/>
       <c r="W38" s="21"/>
       <c r="X38" s="21" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="Y38" s="24" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="Z38" s="21" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="AA38" s="21" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="AB38" s="24" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AC38" s="21"/>
       <c r="AD38" s="21" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="AE38" s="21"/>
       <c r="AF38" s="21"/>
@@ -3866,32 +3742,32 @@
         <v>36</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="21" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="L39" s="21"/>
       <c r="M39" s="21"/>
@@ -3932,26 +3808,26 @@
         <v>36</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H40" s="21"/>
       <c r="I40" s="21" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
@@ -3994,31 +3870,31 @@
         <v>36</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="H41" s="21"/>
       <c r="I41" s="21" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="J41" s="21"/>
       <c r="K41" s="21"/>
       <c r="L41" s="21" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="M41" s="21"/>
       <c r="N41" s="21"/>
@@ -4058,7 +3934,7 @@
         <v>31</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>33</v>
@@ -4117,10 +3993,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
@@ -4142,7 +4018,7 @@
       <c r="T43" s="21"/>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="W43" s="21"/>
       <c r="X43" s="21"/>
@@ -4220,7 +4096,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>33</v>
@@ -4244,7 +4120,7 @@
       <c r="J45" s="21"/>
       <c r="K45" s="21"/>
       <c r="L45" s="21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="M45" s="21"/>
       <c r="N45" s="21"/>
@@ -4281,10 +4157,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
@@ -4306,7 +4182,7 @@
       <c r="T46" s="21"/>
       <c r="U46" s="21"/>
       <c r="V46" s="21" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="W46" s="21"/>
       <c r="X46" s="21"/>
@@ -4333,10 +4209,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -4358,7 +4234,7 @@
       <c r="T47" s="21"/>
       <c r="U47" s="21"/>
       <c r="V47" s="21" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="W47" s="21"/>
       <c r="X47" s="21"/>
@@ -4385,10 +4261,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -4410,7 +4286,7 @@
       <c r="T48" s="21"/>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="W48" s="21"/>
       <c r="X48" s="21"/>
@@ -4549,10 +4425,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4572,7 +4448,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -4601,461 +4477,418 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="21" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>211</v>
-      </c>
       <c r="D3" s="32" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="21" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>225</v>
-      </c>
       <c r="C5" s="31" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="21" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="21" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>240</v>
-      </c>
       <c r="E7" s="17" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="21" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="21" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>254</v>
+        <v>65</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="21" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>266</v>
-      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="20"/>
-      <c r="I10" s="21" t="s">
-        <v>267</v>
-      </c>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>270</v>
-      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="21" t="s">
-        <v>273</v>
-      </c>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>275</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>279</v>
-      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="21" t="s">
-        <v>280</v>
-      </c>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>286</v>
-      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="21" t="s">
-        <v>282</v>
-      </c>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>288</v>
-      </c>
       <c r="D14" s="32" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="21" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="21" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="21" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="21" t="s">
-        <v>315</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5091,40 +4924,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>318</v>
+        <v>285</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>319</v>
+        <v>286</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>320</v>
+        <v>287</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>321</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>322</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="C2" s="38" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-09-24  16-55</v>
+        <v>2024-09-27  0-12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>